<commit_message>
added web-frontend and mobile-frontend to the repo
</commit_message>
<xml_diff>
--- a/ruletadata.xlsx
+++ b/ruletadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\cosas\ruleta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06533A40-FA70-47E8-A606-BD45ED755390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B91F760-EACB-492F-8B84-A33F92BD178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57857837-C85E-4B29-A690-D5CA065EF92E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="236">
   <si>
     <t>Susanita tiene un ratón</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Homer y Bart simpson</t>
   </si>
   <si>
-    <t>el mapa de tesoro</t>
-  </si>
-  <si>
     <t>Bucanero y corsario</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>El escondite inglés</t>
   </si>
   <si>
-    <t>El ajedres y las damas</t>
-  </si>
-  <si>
     <t>tres en raya</t>
   </si>
   <si>
@@ -739,14 +733,31 @@
   </si>
   <si>
     <t xml:space="preserve"> la abeja Maya y Willy</t>
+  </si>
+  <si>
+    <t>El ajedrez y las damas</t>
+  </si>
+  <si>
+    <t>el mapa del tesoro</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -774,8 +785,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702A8EB2-0057-463C-A000-BFD3224B34C3}">
-  <dimension ref="B1:C120"/>
+  <dimension ref="B1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -1115,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1123,15 +1135,15 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1139,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1147,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1155,7 +1167,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1175,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1171,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1179,7 +1191,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -1187,7 +1199,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1207,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -1203,7 +1215,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -1211,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -1219,7 +1231,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -1227,135 +1239,136 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1376,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -1371,7 +1384,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -1379,7 +1392,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -1387,260 +1400,260 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68">
         <v>300</v>
@@ -1648,421 +1661,425 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>79</v>
+        <v>233</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C86" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C93" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>92</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>93</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>94</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C100" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>95</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C101" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
         <v>96</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C102" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>97</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C103" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
         <v>98</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C104" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>99</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C105" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>100</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C106" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+      <c r="D106" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>101</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C107" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>102</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C108" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
         <v>103</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C109" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>104</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C110" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>105</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C111" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>106</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C112" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>107</v>
-      </c>
-      <c r="C111" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>108</v>
-      </c>
-      <c r="C112" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C117" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C118" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C119" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C120" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>